<commit_message>
functional tests for data import
</commit_message>
<xml_diff>
--- a/music_publisher/tests/dataimport.xlsx
+++ b/music_publisher/tests/dataimport.xlsx
@@ -1499,7 +1499,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1561,10 +1561,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3023,8 +3019,8 @@
   </sheetPr>
   <dimension ref="A1:CG4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AS1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AZ3" activeCellId="0" sqref="AZ3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="U3" activeCellId="0" sqref="U3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3304,7 +3300,7 @@
       <c r="O3" s="0" t="s">
         <v>110</v>
       </c>
-      <c r="P3" s="16" t="n">
+      <c r="P3" s="0" t="n">
         <v>0.5</v>
       </c>
       <c r="Q3" s="0" t="s">
@@ -3317,7 +3313,7 @@
         <v>108</v>
       </c>
       <c r="U3" s="0" t="n">
-        <v>297</v>
+        <v>591</v>
       </c>
       <c r="V3" s="0" t="s">
         <v>109</v>
@@ -3469,1877 +3465,1877 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>118</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
-      <c r="P1" s="18"/>
-      <c r="Q1" s="18"/>
-      <c r="R1" s="18"/>
-      <c r="S1" s="18"/>
-      <c r="T1" s="18"/>
-      <c r="U1" s="18"/>
-      <c r="V1" s="18"/>
-      <c r="W1" s="18"/>
-      <c r="X1" s="18"/>
-      <c r="Y1" s="18"/>
-      <c r="Z1" s="18"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="17"/>
+      <c r="S1" s="17"/>
+      <c r="T1" s="17"/>
+      <c r="U1" s="17"/>
+      <c r="V1" s="17"/>
+      <c r="W1" s="17"/>
+      <c r="X1" s="17"/>
+      <c r="Y1" s="17"/>
+      <c r="Z1" s="17"/>
     </row>
     <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18"/>
-      <c r="M2" s="18"/>
-      <c r="N2" s="18"/>
-      <c r="O2" s="18"/>
-      <c r="P2" s="18"/>
-      <c r="Q2" s="18"/>
-      <c r="R2" s="18"/>
-      <c r="S2" s="18"/>
-      <c r="T2" s="18"/>
-      <c r="U2" s="18"/>
-      <c r="V2" s="18"/>
-      <c r="W2" s="18"/>
-      <c r="X2" s="18"/>
-      <c r="Y2" s="18"/>
-      <c r="Z2" s="18"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="17"/>
+      <c r="P2" s="17"/>
+      <c r="Q2" s="17"/>
+      <c r="R2" s="17"/>
+      <c r="S2" s="17"/>
+      <c r="T2" s="17"/>
+      <c r="U2" s="17"/>
+      <c r="V2" s="17"/>
+      <c r="W2" s="17"/>
+      <c r="X2" s="17"/>
+      <c r="Y2" s="17"/>
+      <c r="Z2" s="17"/>
     </row>
     <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="18" t="s">
         <v>122</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-      <c r="K3" s="18"/>
-      <c r="L3" s="18"/>
-      <c r="M3" s="18"/>
-      <c r="N3" s="18"/>
-      <c r="O3" s="18"/>
-      <c r="P3" s="18"/>
-      <c r="Q3" s="18"/>
-      <c r="R3" s="18"/>
-      <c r="S3" s="18"/>
-      <c r="T3" s="18"/>
-      <c r="U3" s="18"/>
-      <c r="V3" s="18"/>
-      <c r="W3" s="18"/>
-      <c r="X3" s="18"/>
-      <c r="Y3" s="18"/>
-      <c r="Z3" s="18"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="17"/>
+      <c r="M3" s="17"/>
+      <c r="N3" s="17"/>
+      <c r="O3" s="17"/>
+      <c r="P3" s="17"/>
+      <c r="Q3" s="17"/>
+      <c r="R3" s="17"/>
+      <c r="S3" s="17"/>
+      <c r="T3" s="17"/>
+      <c r="U3" s="17"/>
+      <c r="V3" s="17"/>
+      <c r="W3" s="17"/>
+      <c r="X3" s="17"/>
+      <c r="Y3" s="17"/>
+      <c r="Z3" s="17"/>
     </row>
     <row r="4" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="17" t="s">
         <v>126</v>
       </c>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="18"/>
-      <c r="L4" s="18"/>
-      <c r="M4" s="18"/>
-      <c r="N4" s="18"/>
-      <c r="O4" s="18"/>
-      <c r="P4" s="18"/>
-      <c r="Q4" s="18"/>
-      <c r="R4" s="18"/>
-      <c r="S4" s="18"/>
-      <c r="T4" s="18"/>
-      <c r="U4" s="18"/>
-      <c r="V4" s="18"/>
-      <c r="W4" s="18"/>
-      <c r="X4" s="18"/>
-      <c r="Y4" s="18"/>
-      <c r="Z4" s="18"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="17"/>
+      <c r="L4" s="17"/>
+      <c r="M4" s="17"/>
+      <c r="N4" s="17"/>
+      <c r="O4" s="17"/>
+      <c r="P4" s="17"/>
+      <c r="Q4" s="17"/>
+      <c r="R4" s="17"/>
+      <c r="S4" s="17"/>
+      <c r="T4" s="17"/>
+      <c r="U4" s="17"/>
+      <c r="V4" s="17"/>
+      <c r="W4" s="17"/>
+      <c r="X4" s="17"/>
+      <c r="Y4" s="17"/>
+      <c r="Z4" s="17"/>
     </row>
     <row r="5" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="17" t="s">
         <v>128</v>
       </c>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18"/>
-      <c r="L5" s="18"/>
-      <c r="M5" s="18"/>
-      <c r="N5" s="18"/>
-      <c r="O5" s="18"/>
-      <c r="P5" s="18"/>
-      <c r="Q5" s="18"/>
-      <c r="R5" s="18"/>
-      <c r="S5" s="18"/>
-      <c r="T5" s="18"/>
-      <c r="U5" s="18"/>
-      <c r="V5" s="18"/>
-      <c r="W5" s="18"/>
-      <c r="X5" s="18"/>
-      <c r="Y5" s="18"/>
-      <c r="Z5" s="18"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="17"/>
+      <c r="L5" s="17"/>
+      <c r="M5" s="17"/>
+      <c r="N5" s="17"/>
+      <c r="O5" s="17"/>
+      <c r="P5" s="17"/>
+      <c r="Q5" s="17"/>
+      <c r="R5" s="17"/>
+      <c r="S5" s="17"/>
+      <c r="T5" s="17"/>
+      <c r="U5" s="17"/>
+      <c r="V5" s="17"/>
+      <c r="W5" s="17"/>
+      <c r="X5" s="17"/>
+      <c r="Y5" s="17"/>
+      <c r="Z5" s="17"/>
     </row>
     <row r="6" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="18"/>
-      <c r="M6" s="18"/>
-      <c r="N6" s="18"/>
-      <c r="O6" s="18"/>
-      <c r="P6" s="18"/>
-      <c r="Q6" s="18"/>
-      <c r="R6" s="18"/>
-      <c r="S6" s="18"/>
-      <c r="T6" s="18"/>
-      <c r="U6" s="18"/>
-      <c r="V6" s="18"/>
-      <c r="W6" s="18"/>
-      <c r="X6" s="18"/>
-      <c r="Y6" s="18"/>
-      <c r="Z6" s="18"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="17"/>
+      <c r="L6" s="17"/>
+      <c r="M6" s="17"/>
+      <c r="N6" s="17"/>
+      <c r="O6" s="17"/>
+      <c r="P6" s="17"/>
+      <c r="Q6" s="17"/>
+      <c r="R6" s="17"/>
+      <c r="S6" s="17"/>
+      <c r="T6" s="17"/>
+      <c r="U6" s="17"/>
+      <c r="V6" s="17"/>
+      <c r="W6" s="17"/>
+      <c r="X6" s="17"/>
+      <c r="Y6" s="17"/>
+      <c r="Z6" s="17"/>
     </row>
     <row r="7" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="18" t="s">
         <v>131</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="17" t="s">
         <v>132</v>
       </c>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="18"/>
-      <c r="L7" s="18"/>
-      <c r="M7" s="18"/>
-      <c r="N7" s="18"/>
-      <c r="O7" s="18"/>
-      <c r="P7" s="18"/>
-      <c r="Q7" s="18"/>
-      <c r="R7" s="18"/>
-      <c r="S7" s="18"/>
-      <c r="T7" s="18"/>
-      <c r="U7" s="18"/>
-      <c r="V7" s="18"/>
-      <c r="W7" s="18"/>
-      <c r="X7" s="18"/>
-      <c r="Y7" s="18"/>
-      <c r="Z7" s="18"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="17"/>
+      <c r="L7" s="17"/>
+      <c r="M7" s="17"/>
+      <c r="N7" s="17"/>
+      <c r="O7" s="17"/>
+      <c r="P7" s="17"/>
+      <c r="Q7" s="17"/>
+      <c r="R7" s="17"/>
+      <c r="S7" s="17"/>
+      <c r="T7" s="17"/>
+      <c r="U7" s="17"/>
+      <c r="V7" s="17"/>
+      <c r="W7" s="17"/>
+      <c r="X7" s="17"/>
+      <c r="Y7" s="17"/>
+      <c r="Z7" s="17"/>
     </row>
     <row r="8" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="17" t="s">
         <v>133</v>
       </c>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="18"/>
-      <c r="L8" s="18"/>
-      <c r="M8" s="18"/>
-      <c r="N8" s="18"/>
-      <c r="O8" s="18"/>
-      <c r="P8" s="18"/>
-      <c r="Q8" s="18"/>
-      <c r="R8" s="18"/>
-      <c r="S8" s="18"/>
-      <c r="T8" s="18"/>
-      <c r="U8" s="18"/>
-      <c r="V8" s="18"/>
-      <c r="W8" s="18"/>
-      <c r="X8" s="18"/>
-      <c r="Y8" s="18"/>
-      <c r="Z8" s="18"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="17"/>
+      <c r="L8" s="17"/>
+      <c r="M8" s="17"/>
+      <c r="N8" s="17"/>
+      <c r="O8" s="17"/>
+      <c r="P8" s="17"/>
+      <c r="Q8" s="17"/>
+      <c r="R8" s="17"/>
+      <c r="S8" s="17"/>
+      <c r="T8" s="17"/>
+      <c r="U8" s="17"/>
+      <c r="V8" s="17"/>
+      <c r="W8" s="17"/>
+      <c r="X8" s="17"/>
+      <c r="Y8" s="17"/>
+      <c r="Z8" s="17"/>
     </row>
     <row r="9" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="18"/>
-      <c r="L9" s="18"/>
-      <c r="M9" s="18"/>
-      <c r="N9" s="18"/>
-      <c r="O9" s="18"/>
-      <c r="P9" s="18"/>
-      <c r="Q9" s="18"/>
-      <c r="R9" s="18"/>
-      <c r="S9" s="18"/>
-      <c r="T9" s="18"/>
-      <c r="U9" s="18"/>
-      <c r="V9" s="18"/>
-      <c r="W9" s="18"/>
-      <c r="X9" s="18"/>
-      <c r="Y9" s="18"/>
-      <c r="Z9" s="18"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="17"/>
+      <c r="N9" s="17"/>
+      <c r="O9" s="17"/>
+      <c r="P9" s="17"/>
+      <c r="Q9" s="17"/>
+      <c r="R9" s="17"/>
+      <c r="S9" s="17"/>
+      <c r="T9" s="17"/>
+      <c r="U9" s="17"/>
+      <c r="V9" s="17"/>
+      <c r="W9" s="17"/>
+      <c r="X9" s="17"/>
+      <c r="Y9" s="17"/>
+      <c r="Z9" s="17"/>
     </row>
     <row r="10" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="19"/>
-      <c r="B10" s="18" t="s">
+      <c r="A10" s="18"/>
+      <c r="B10" s="17" t="s">
         <v>135</v>
       </c>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="18"/>
-      <c r="L10" s="18"/>
-      <c r="M10" s="18"/>
-      <c r="N10" s="18"/>
-      <c r="O10" s="18"/>
-      <c r="P10" s="18"/>
-      <c r="Q10" s="18"/>
-      <c r="R10" s="18"/>
-      <c r="S10" s="18"/>
-      <c r="T10" s="18"/>
-      <c r="U10" s="18"/>
-      <c r="V10" s="18"/>
-      <c r="W10" s="18"/>
-      <c r="X10" s="18"/>
-      <c r="Y10" s="18"/>
-      <c r="Z10" s="18"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="17"/>
+      <c r="N10" s="17"/>
+      <c r="O10" s="17"/>
+      <c r="P10" s="17"/>
+      <c r="Q10" s="17"/>
+      <c r="R10" s="17"/>
+      <c r="S10" s="17"/>
+      <c r="T10" s="17"/>
+      <c r="U10" s="17"/>
+      <c r="V10" s="17"/>
+      <c r="W10" s="17"/>
+      <c r="X10" s="17"/>
+      <c r="Y10" s="17"/>
+      <c r="Z10" s="17"/>
     </row>
     <row r="11" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="19"/>
-      <c r="B11" s="18" t="s">
+      <c r="A11" s="18"/>
+      <c r="B11" s="17" t="s">
         <v>136</v>
       </c>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="18"/>
-      <c r="L11" s="18"/>
-      <c r="M11" s="18"/>
-      <c r="N11" s="18"/>
-      <c r="O11" s="18"/>
-      <c r="P11" s="18"/>
-      <c r="Q11" s="18"/>
-      <c r="R11" s="18"/>
-      <c r="S11" s="18"/>
-      <c r="T11" s="18"/>
-      <c r="U11" s="18"/>
-      <c r="V11" s="18"/>
-      <c r="W11" s="18"/>
-      <c r="X11" s="18"/>
-      <c r="Y11" s="18"/>
-      <c r="Z11" s="18"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="17"/>
+      <c r="L11" s="17"/>
+      <c r="M11" s="17"/>
+      <c r="N11" s="17"/>
+      <c r="O11" s="17"/>
+      <c r="P11" s="17"/>
+      <c r="Q11" s="17"/>
+      <c r="R11" s="17"/>
+      <c r="S11" s="17"/>
+      <c r="T11" s="17"/>
+      <c r="U11" s="17"/>
+      <c r="V11" s="17"/>
+      <c r="W11" s="17"/>
+      <c r="X11" s="17"/>
+      <c r="Y11" s="17"/>
+      <c r="Z11" s="17"/>
     </row>
     <row r="12" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="18"/>
-      <c r="B12" s="18" t="s">
+      <c r="A12" s="17"/>
+      <c r="B12" s="17" t="s">
         <v>137</v>
       </c>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18"/>
-      <c r="K12" s="18"/>
-      <c r="L12" s="18"/>
-      <c r="M12" s="18"/>
-      <c r="N12" s="18"/>
-      <c r="O12" s="18"/>
-      <c r="P12" s="18"/>
-      <c r="Q12" s="18"/>
-      <c r="R12" s="18"/>
-      <c r="S12" s="18"/>
-      <c r="T12" s="18"/>
-      <c r="U12" s="18"/>
-      <c r="V12" s="18"/>
-      <c r="W12" s="18"/>
-      <c r="X12" s="18"/>
-      <c r="Y12" s="18"/>
-      <c r="Z12" s="18"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="17"/>
+      <c r="L12" s="17"/>
+      <c r="M12" s="17"/>
+      <c r="N12" s="17"/>
+      <c r="O12" s="17"/>
+      <c r="P12" s="17"/>
+      <c r="Q12" s="17"/>
+      <c r="R12" s="17"/>
+      <c r="S12" s="17"/>
+      <c r="T12" s="17"/>
+      <c r="U12" s="17"/>
+      <c r="V12" s="17"/>
+      <c r="W12" s="17"/>
+      <c r="X12" s="17"/>
+      <c r="Y12" s="17"/>
+      <c r="Z12" s="17"/>
     </row>
     <row r="13" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="17" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B14" s="18" t="s">
+      <c r="B14" s="17" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="17" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B16" s="18" t="s">
+      <c r="B16" s="17" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B17" s="18" t="s">
+      <c r="B17" s="17" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="17" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="17" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B20" s="18" t="s">
+      <c r="B20" s="17" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B21" s="18" t="s">
+      <c r="B21" s="17" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B22" s="18" t="s">
+      <c r="B22" s="17" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B23" s="18" t="s">
+      <c r="B23" s="17" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B24" s="18" t="s">
+      <c r="B24" s="17" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B25" s="18" t="s">
+      <c r="B25" s="17" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B26" s="18" t="s">
+      <c r="B26" s="17" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B27" s="18" t="s">
+      <c r="B27" s="17" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B28" s="18" t="s">
+      <c r="B28" s="17" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B29" s="18" t="s">
+      <c r="B29" s="17" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B30" s="18" t="s">
+      <c r="B30" s="17" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B31" s="18" t="s">
+      <c r="B31" s="17" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B32" s="18" t="s">
+      <c r="B32" s="17" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B33" s="18" t="s">
+      <c r="B33" s="17" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B34" s="18" t="s">
+      <c r="B34" s="17" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B35" s="18" t="s">
+      <c r="B35" s="17" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B36" s="18" t="s">
+      <c r="B36" s="17" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B37" s="18" t="s">
+      <c r="B37" s="17" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B38" s="18" t="s">
+      <c r="B38" s="17" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B39" s="18" t="s">
+      <c r="B39" s="17" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B40" s="18" t="s">
+      <c r="B40" s="17" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B41" s="18" t="s">
+      <c r="B41" s="17" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B42" s="18" t="s">
+      <c r="B42" s="17" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B43" s="18" t="s">
+      <c r="B43" s="17" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B44" s="18" t="s">
+      <c r="B44" s="17" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B45" s="18" t="s">
+      <c r="B45" s="17" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B46" s="18" t="s">
+      <c r="B46" s="17" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B47" s="18" t="s">
+      <c r="B47" s="17" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B48" s="18" t="s">
+      <c r="B48" s="17" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B49" s="18" t="s">
+      <c r="B49" s="17" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B50" s="18" t="s">
+      <c r="B50" s="17" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B51" s="18" t="s">
+      <c r="B51" s="17" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B52" s="18" t="s">
+      <c r="B52" s="17" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B53" s="18" t="s">
+      <c r="B53" s="17" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B54" s="18" t="s">
+      <c r="B54" s="17" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B55" s="18" t="s">
+      <c r="B55" s="17" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B56" s="18" t="s">
+      <c r="B56" s="17" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B57" s="18" t="s">
+      <c r="B57" s="17" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B58" s="18" t="s">
+      <c r="B58" s="17" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B59" s="18" t="s">
+      <c r="B59" s="17" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B60" s="18" t="s">
+      <c r="B60" s="17" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B61" s="18" t="s">
+      <c r="B61" s="17" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B62" s="18" t="s">
+      <c r="B62" s="17" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B63" s="18" t="s">
+      <c r="B63" s="17" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B64" s="18" t="s">
+      <c r="B64" s="17" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B65" s="18" t="s">
+      <c r="B65" s="17" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B66" s="18" t="s">
+      <c r="B66" s="17" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B67" s="18" t="s">
+      <c r="B67" s="17" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B68" s="18" t="s">
+      <c r="B68" s="17" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B69" s="18" t="s">
+      <c r="B69" s="17" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B70" s="18" t="s">
+      <c r="B70" s="17" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B71" s="18" t="s">
+      <c r="B71" s="17" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B72" s="18" t="s">
+      <c r="B72" s="17" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B73" s="18" t="s">
+      <c r="B73" s="17" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B74" s="18" t="s">
+      <c r="B74" s="17" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B75" s="18" t="s">
+      <c r="B75" s="17" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B76" s="18" t="s">
+      <c r="B76" s="17" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B77" s="18" t="s">
+      <c r="B77" s="17" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B78" s="18" t="s">
+      <c r="B78" s="17" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B79" s="18" t="s">
+      <c r="B79" s="17" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B80" s="18" t="s">
+      <c r="B80" s="17" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B81" s="18" t="s">
+      <c r="B81" s="17" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B82" s="18" t="s">
+      <c r="B82" s="17" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B83" s="18" t="s">
+      <c r="B83" s="17" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B84" s="18" t="s">
+      <c r="B84" s="17" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B85" s="18" t="s">
+      <c r="B85" s="17" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B86" s="18" t="s">
+      <c r="B86" s="17" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B87" s="18" t="s">
+      <c r="B87" s="17" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B88" s="18" t="s">
+      <c r="B88" s="17" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B89" s="18" t="s">
+      <c r="B89" s="17" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B90" s="18" t="s">
+      <c r="B90" s="17" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B91" s="18" t="s">
+      <c r="B91" s="17" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B92" s="18" t="s">
+      <c r="B92" s="17" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B93" s="18" t="s">
+      <c r="B93" s="17" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B94" s="18" t="s">
+      <c r="B94" s="17" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B95" s="18" t="s">
+      <c r="B95" s="17" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B96" s="18" t="s">
+      <c r="B96" s="17" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B97" s="18" t="s">
+      <c r="B97" s="17" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B98" s="18" t="s">
+      <c r="B98" s="17" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B99" s="18" t="s">
+      <c r="B99" s="17" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B100" s="18" t="s">
+      <c r="B100" s="17" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B101" s="18" t="s">
+      <c r="B101" s="17" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B102" s="18" t="s">
+      <c r="B102" s="17" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B103" s="18" t="s">
+      <c r="B103" s="17" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B104" s="18" t="s">
+      <c r="B104" s="17" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B105" s="18" t="s">
+      <c r="B105" s="17" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B106" s="18" t="s">
+      <c r="B106" s="17" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B107" s="18" t="s">
+      <c r="B107" s="17" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B108" s="18" t="s">
+      <c r="B108" s="17" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B109" s="18" t="s">
+      <c r="B109" s="17" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B110" s="18" t="s">
+      <c r="B110" s="17" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B111" s="18" t="s">
+      <c r="B111" s="17" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B112" s="18" t="s">
+      <c r="B112" s="17" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B113" s="18" t="s">
+      <c r="B113" s="17" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B114" s="18" t="s">
+      <c r="B114" s="17" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B115" s="18" t="s">
+      <c r="B115" s="17" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B116" s="18" t="s">
+      <c r="B116" s="17" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B117" s="18" t="s">
+      <c r="B117" s="17" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B118" s="18" t="s">
+      <c r="B118" s="17" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B119" s="18" t="s">
+      <c r="B119" s="17" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B120" s="18" t="s">
+      <c r="B120" s="17" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B121" s="18" t="s">
+      <c r="B121" s="17" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B122" s="18" t="s">
+      <c r="B122" s="17" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B123" s="18" t="s">
+      <c r="B123" s="17" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B124" s="18" t="s">
+      <c r="B124" s="17" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B125" s="18" t="s">
+      <c r="B125" s="17" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B126" s="18" t="s">
+      <c r="B126" s="17" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B127" s="18" t="s">
+      <c r="B127" s="17" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B128" s="18" t="s">
+      <c r="B128" s="17" t="s">
         <v>253</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B129" s="18" t="s">
+      <c r="B129" s="17" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B130" s="18" t="s">
+      <c r="B130" s="17" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B131" s="18" t="s">
+      <c r="B131" s="17" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B132" s="18" t="s">
+      <c r="B132" s="17" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B133" s="18" t="s">
+      <c r="B133" s="17" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B134" s="18" t="s">
+      <c r="B134" s="17" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B135" s="18" t="s">
+      <c r="B135" s="17" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B136" s="18" t="s">
+      <c r="B136" s="17" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B137" s="18" t="s">
+      <c r="B137" s="17" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B138" s="18" t="s">
+      <c r="B138" s="17" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B139" s="18" t="s">
+      <c r="B139" s="17" t="s">
         <v>264</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B140" s="18" t="s">
+      <c r="B140" s="17" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B141" s="18" t="s">
+      <c r="B141" s="17" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B142" s="18" t="s">
+      <c r="B142" s="17" t="s">
         <v>267</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B143" s="18" t="s">
+      <c r="B143" s="17" t="s">
         <v>268</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B144" s="18" t="s">
+      <c r="B144" s="17" t="s">
         <v>269</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B145" s="18" t="s">
+      <c r="B145" s="17" t="s">
         <v>270</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B146" s="18" t="s">
+      <c r="B146" s="17" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B147" s="18" t="s">
+      <c r="B147" s="17" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B148" s="18" t="s">
+      <c r="B148" s="17" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B149" s="18" t="s">
+      <c r="B149" s="17" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B150" s="18" t="s">
+      <c r="B150" s="17" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B151" s="18" t="s">
+      <c r="B151" s="17" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B152" s="18" t="s">
+      <c r="B152" s="17" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B153" s="18" t="s">
+      <c r="B153" s="17" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B154" s="18" t="s">
+      <c r="B154" s="17" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B155" s="18" t="s">
+      <c r="B155" s="17" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B156" s="18" t="s">
+      <c r="B156" s="17" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B157" s="18" t="s">
+      <c r="B157" s="17" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B158" s="18" t="s">
+      <c r="B158" s="17" t="s">
         <v>283</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B159" s="18" t="s">
+      <c r="B159" s="17" t="s">
         <v>284</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B160" s="18" t="s">
+      <c r="B160" s="17" t="s">
         <v>285</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B161" s="18" t="s">
+      <c r="B161" s="17" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B162" s="18" t="s">
+      <c r="B162" s="17" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B163" s="18" t="s">
+      <c r="B163" s="17" t="s">
         <v>288</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B164" s="18" t="s">
+      <c r="B164" s="17" t="s">
         <v>289</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B165" s="18" t="s">
+      <c r="B165" s="17" t="s">
         <v>290</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B166" s="18" t="s">
+      <c r="B166" s="17" t="s">
         <v>291</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B167" s="18" t="s">
+      <c r="B167" s="17" t="s">
         <v>292</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B168" s="18" t="s">
+      <c r="B168" s="17" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B169" s="18" t="s">
+      <c r="B169" s="17" t="s">
         <v>294</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B170" s="18" t="s">
+      <c r="B170" s="17" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B171" s="18" t="s">
+      <c r="B171" s="17" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B172" s="18" t="s">
+      <c r="B172" s="17" t="s">
         <v>297</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B173" s="18" t="s">
+      <c r="B173" s="17" t="s">
         <v>298</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B174" s="18" t="s">
+      <c r="B174" s="17" t="s">
         <v>299</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B175" s="18" t="s">
+      <c r="B175" s="17" t="s">
         <v>300</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B176" s="18" t="s">
+      <c r="B176" s="17" t="s">
         <v>301</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B177" s="18" t="s">
+      <c r="B177" s="17" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B178" s="18" t="s">
+      <c r="B178" s="17" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B179" s="18" t="s">
+      <c r="B179" s="17" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B180" s="18" t="s">
+      <c r="B180" s="17" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B181" s="18" t="s">
+      <c r="B181" s="17" t="s">
         <v>306</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B182" s="18" t="s">
+      <c r="B182" s="17" t="s">
         <v>307</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B183" s="18" t="s">
+      <c r="B183" s="17" t="s">
         <v>308</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B184" s="18" t="s">
+      <c r="B184" s="17" t="s">
         <v>309</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B185" s="18" t="s">
+      <c r="B185" s="17" t="s">
         <v>310</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B186" s="18" t="s">
+      <c r="B186" s="17" t="s">
         <v>311</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B187" s="18" t="s">
+      <c r="B187" s="17" t="s">
         <v>312</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B188" s="18" t="s">
+      <c r="B188" s="17" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B189" s="18" t="s">
+      <c r="B189" s="17" t="s">
         <v>314</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B190" s="18" t="s">
+      <c r="B190" s="17" t="s">
         <v>315</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B191" s="18" t="s">
+      <c r="B191" s="17" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B192" s="18" t="s">
+      <c r="B192" s="17" t="s">
         <v>317</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B193" s="18" t="s">
+      <c r="B193" s="17" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B194" s="18" t="s">
+      <c r="B194" s="17" t="s">
         <v>319</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B195" s="18" t="s">
+      <c r="B195" s="17" t="s">
         <v>320</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B196" s="18" t="s">
+      <c r="B196" s="17" t="s">
         <v>321</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B197" s="18" t="s">
+      <c r="B197" s="17" t="s">
         <v>322</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B198" s="18" t="s">
+      <c r="B198" s="17" t="s">
         <v>323</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B199" s="18" t="s">
+      <c r="B199" s="17" t="s">
         <v>324</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B200" s="18" t="s">
+      <c r="B200" s="17" t="s">
         <v>325</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B201" s="18" t="s">
+      <c r="B201" s="17" t="s">
         <v>326</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B202" s="18" t="s">
+      <c r="B202" s="17" t="s">
         <v>327</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B203" s="18" t="s">
+      <c r="B203" s="17" t="s">
         <v>328</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B204" s="18" t="s">
+      <c r="B204" s="17" t="s">
         <v>329</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B205" s="18" t="s">
+      <c r="B205" s="17" t="s">
         <v>330</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B206" s="18" t="s">
+      <c r="B206" s="17" t="s">
         <v>331</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B207" s="18" t="s">
+      <c r="B207" s="17" t="s">
         <v>332</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B208" s="18" t="s">
+      <c r="B208" s="17" t="s">
         <v>333</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B209" s="18" t="s">
+      <c r="B209" s="17" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B210" s="18" t="s">
+      <c r="B210" s="17" t="s">
         <v>335</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B211" s="18" t="s">
+      <c r="B211" s="17" t="s">
         <v>336</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B212" s="18" t="s">
+      <c r="B212" s="17" t="s">
         <v>337</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B213" s="18" t="s">
+      <c r="B213" s="17" t="s">
         <v>338</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B214" s="18" t="s">
+      <c r="B214" s="17" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B215" s="18" t="s">
+      <c r="B215" s="17" t="s">
         <v>340</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B216" s="18" t="s">
+      <c r="B216" s="17" t="s">
         <v>341</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B217" s="18" t="s">
+      <c r="B217" s="17" t="s">
         <v>342</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B218" s="20" t="s">
+      <c r="B218" s="19" t="s">
         <v>343</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B219" s="20" t="s">
+      <c r="B219" s="19" t="s">
         <v>344</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B220" s="20" t="s">
+      <c r="B220" s="19" t="s">
         <v>345</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B221" s="20" t="s">
+      <c r="B221" s="19" t="s">
         <v>346</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B222" s="20" t="s">
+      <c r="B222" s="19" t="s">
         <v>347</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B223" s="20" t="s">
+      <c r="B223" s="19" t="s">
         <v>348</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B224" s="20" t="s">
+      <c r="B224" s="19" t="s">
         <v>349</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B225" s="20" t="s">
+      <c r="B225" s="19" t="s">
         <v>350</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B226" s="20" t="s">
+      <c r="B226" s="19" t="s">
         <v>351</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B227" s="20" t="s">
+      <c r="B227" s="19" t="s">
         <v>352</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B228" s="20" t="s">
+      <c r="B228" s="19" t="s">
         <v>353</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B229" s="20" t="s">
+      <c r="B229" s="19" t="s">
         <v>354</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B230" s="20" t="s">
+      <c r="B230" s="19" t="s">
         <v>355</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B231" s="20" t="s">
+      <c r="B231" s="19" t="s">
         <v>356</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B232" s="20" t="s">
+      <c r="B232" s="19" t="s">
         <v>357</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B233" s="20" t="s">
+      <c r="B233" s="19" t="s">
         <v>358</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B234" s="20" t="s">
+      <c r="B234" s="19" t="s">
         <v>359</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B235" s="20" t="s">
+      <c r="B235" s="19" t="s">
         <v>360</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B236" s="20" t="s">
+      <c r="B236" s="19" t="s">
         <v>361</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B237" s="20" t="s">
+      <c r="B237" s="19" t="s">
         <v>362</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B238" s="20" t="s">
+      <c r="B238" s="19" t="s">
         <v>363</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B239" s="20" t="s">
+      <c r="B239" s="19" t="s">
         <v>364</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B240" s="20" t="s">
+      <c r="B240" s="19" t="s">
         <v>365</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B241" s="20" t="s">
+      <c r="B241" s="19" t="s">
         <v>366</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B242" s="20" t="s">
+      <c r="B242" s="19" t="s">
         <v>367</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B243" s="20" t="s">
+      <c r="B243" s="19" t="s">
         <v>368</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B244" s="20" t="s">
+      <c r="B244" s="19" t="s">
         <v>369</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B245" s="20" t="s">
+      <c r="B245" s="19" t="s">
         <v>370</v>
       </c>
     </row>
     <row r="246" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B246" s="20" t="s">
+      <c r="B246" s="19" t="s">
         <v>371</v>
       </c>
     </row>
     <row r="247" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B247" s="20" t="s">
+      <c r="B247" s="19" t="s">
         <v>372</v>
       </c>
     </row>
     <row r="248" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B248" s="20" t="s">
+      <c r="B248" s="19" t="s">
         <v>373</v>
       </c>
     </row>
     <row r="249" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B249" s="20" t="s">
+      <c r="B249" s="19" t="s">
         <v>374</v>
       </c>
     </row>
     <row r="250" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B250" s="20" t="s">
+      <c r="B250" s="19" t="s">
         <v>375</v>
       </c>
     </row>
     <row r="251" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B251" s="20" t="s">
+      <c r="B251" s="19" t="s">
         <v>376</v>
       </c>
     </row>
     <row r="252" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B252" s="20" t="s">
+      <c r="B252" s="19" t="s">
         <v>377</v>
       </c>
     </row>
     <row r="253" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B253" s="20" t="s">
+      <c r="B253" s="19" t="s">
         <v>378</v>
       </c>
     </row>
     <row r="254" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B254" s="20" t="s">
+      <c r="B254" s="19" t="s">
         <v>379</v>
       </c>
     </row>
     <row r="255" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B255" s="20" t="s">
+      <c r="B255" s="19" t="s">
         <v>380</v>
       </c>
     </row>
     <row r="256" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B256" s="20" t="s">
+      <c r="B256" s="19" t="s">
         <v>381</v>
       </c>
     </row>
     <row r="257" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B257" s="20" t="s">
+      <c r="B257" s="19" t="s">
         <v>382</v>
       </c>
     </row>
     <row r="258" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B258" s="20" t="s">
+      <c r="B258" s="19" t="s">
         <v>383</v>
       </c>
     </row>
     <row r="259" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B259" s="20" t="s">
+      <c r="B259" s="19" t="s">
         <v>384</v>
       </c>
     </row>
     <row r="260" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B260" s="20" t="s">
+      <c r="B260" s="19" t="s">
         <v>385</v>
       </c>
     </row>
     <row r="261" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B261" s="20" t="s">
+      <c r="B261" s="19" t="s">
         <v>386</v>
       </c>
     </row>
     <row r="262" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B262" s="20" t="s">
+      <c r="B262" s="19" t="s">
         <v>387</v>
       </c>
     </row>
     <row r="263" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B263" s="20" t="s">
+      <c r="B263" s="19" t="s">
         <v>388</v>
       </c>
     </row>
     <row r="264" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B264" s="20" t="s">
+      <c r="B264" s="19" t="s">
         <v>389</v>
       </c>
     </row>
     <row r="265" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B265" s="20" t="s">
+      <c r="B265" s="19" t="s">
         <v>390</v>
       </c>
     </row>
     <row r="266" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B266" s="20" t="s">
+      <c r="B266" s="19" t="s">
         <v>391</v>
       </c>
     </row>
     <row r="267" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B267" s="20" t="s">
+      <c r="B267" s="19" t="s">
         <v>392</v>
       </c>
     </row>
     <row r="268" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B268" s="20" t="s">
+      <c r="B268" s="19" t="s">
         <v>393</v>
       </c>
     </row>
     <row r="269" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B269" s="20" t="s">
+      <c r="B269" s="19" t="s">
         <v>394</v>
       </c>
     </row>
     <row r="270" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B270" s="20" t="s">
+      <c r="B270" s="19" t="s">
         <v>395</v>
       </c>
     </row>
     <row r="271" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B271" s="20" t="s">
+      <c r="B271" s="19" t="s">
         <v>396</v>
       </c>
     </row>
     <row r="272" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B272" s="20" t="s">
+      <c r="B272" s="19" t="s">
         <v>397</v>
       </c>
     </row>
     <row r="273" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B273" s="20" t="s">
+      <c r="B273" s="19" t="s">
         <v>398</v>
       </c>
     </row>
     <row r="274" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B274" s="20" t="s">
+      <c r="B274" s="19" t="s">
         <v>399</v>
       </c>
     </row>
     <row r="275" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B275" s="20" t="s">
+      <c r="B275" s="19" t="s">
         <v>400</v>
       </c>
     </row>
     <row r="276" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B276" s="20" t="s">
+      <c r="B276" s="19" t="s">
         <v>401</v>
       </c>
     </row>
     <row r="277" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B277" s="20" t="s">
+      <c r="B277" s="19" t="s">
         <v>402</v>
       </c>
     </row>
     <row r="278" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B278" s="20" t="s">
+      <c r="B278" s="19" t="s">
         <v>403</v>
       </c>
     </row>
     <row r="279" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B279" s="20" t="s">
+      <c r="B279" s="19" t="s">
         <v>404</v>
       </c>
     </row>
     <row r="280" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B280" s="20" t="s">
+      <c r="B280" s="19" t="s">
         <v>405</v>
       </c>
     </row>
     <row r="281" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B281" s="20" t="s">
+      <c r="B281" s="19" t="s">
         <v>406</v>
       </c>
     </row>
     <row r="282" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B282" s="20" t="s">
+      <c r="B282" s="19" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="283" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B283" s="20" t="s">
+      <c r="B283" s="19" t="s">
         <v>408</v>
       </c>
     </row>
     <row r="284" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B284" s="20" t="s">
+      <c r="B284" s="19" t="s">
         <v>409</v>
       </c>
     </row>
     <row r="285" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B285" s="20" t="s">
+      <c r="B285" s="19" t="s">
         <v>410</v>
       </c>
     </row>
     <row r="286" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B286" s="20" t="s">
+      <c r="B286" s="19" t="s">
         <v>411</v>
       </c>
     </row>
     <row r="287" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B287" s="20" t="s">
+      <c r="B287" s="19" t="s">
         <v>412</v>
       </c>
     </row>
     <row r="288" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B288" s="20" t="s">
+      <c r="B288" s="19" t="s">
         <v>413</v>
       </c>
     </row>
     <row r="289" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B289" s="20" t="s">
+      <c r="B289" s="19" t="s">
         <v>414</v>
       </c>
     </row>
     <row r="290" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B290" s="20" t="s">
+      <c r="B290" s="19" t="s">
         <v>415</v>
       </c>
     </row>
     <row r="291" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B291" s="20" t="s">
+      <c r="B291" s="19" t="s">
         <v>416</v>
       </c>
     </row>
     <row r="292" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B292" s="20" t="s">
+      <c r="B292" s="19" t="s">
         <v>417</v>
       </c>
     </row>
     <row r="293" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B293" s="20" t="s">
+      <c r="B293" s="19" t="s">
         <v>418</v>
       </c>
     </row>
     <row r="294" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B294" s="20" t="s">
+      <c r="B294" s="19" t="s">
         <v>419</v>
       </c>
     </row>
     <row r="295" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B295" s="20" t="s">
+      <c r="B295" s="19" t="s">
         <v>420</v>
       </c>
     </row>
     <row r="296" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B296" s="20" t="s">
+      <c r="B296" s="19" t="s">
         <v>421</v>
       </c>
     </row>
     <row r="297" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B297" s="20" t="s">
+      <c r="B297" s="19" t="s">
         <v>422</v>
       </c>
     </row>
     <row r="298" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B298" s="20" t="s">
+      <c r="B298" s="19" t="s">
         <v>423</v>
       </c>
     </row>
     <row r="299" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B299" s="20" t="s">
+      <c r="B299" s="19" t="s">
         <v>424</v>
       </c>
     </row>
     <row r="300" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B300" s="20" t="s">
+      <c r="B300" s="19" t="s">
         <v>425</v>
       </c>
     </row>
     <row r="301" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B301" s="20" t="s">
+      <c r="B301" s="19" t="s">
         <v>426</v>
       </c>
     </row>
     <row r="302" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B302" s="20" t="s">
+      <c r="B302" s="19" t="s">
         <v>427</v>
       </c>
     </row>
     <row r="303" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B303" s="20" t="s">
+      <c r="B303" s="19" t="s">
         <v>428</v>
       </c>
     </row>
     <row r="304" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B304" s="20" t="s">
+      <c r="B304" s="19" t="s">
         <v>429</v>
       </c>
     </row>
     <row r="305" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B305" s="20" t="s">
+      <c r="B305" s="19" t="s">
         <v>430</v>
       </c>
     </row>
     <row r="306" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B306" s="20" t="s">
+      <c r="B306" s="19" t="s">
         <v>431</v>
       </c>
     </row>
     <row r="307" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B307" s="20" t="s">
+      <c r="B307" s="19" t="s">
         <v>432</v>
       </c>
     </row>
     <row r="308" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B308" s="20" t="s">
+      <c r="B308" s="19" t="s">
         <v>433</v>
       </c>
     </row>
     <row r="309" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B309" s="20" t="s">
+      <c r="B309" s="19" t="s">
         <v>434</v>
       </c>
     </row>
     <row r="310" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B310" s="20" t="s">
+      <c r="B310" s="19" t="s">
         <v>435</v>
       </c>
     </row>
     <row r="311" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B311" s="20" t="s">
+      <c r="B311" s="19" t="s">
         <v>436</v>
       </c>
     </row>

</xml_diff>